<commit_message>
initial logic of cash-flow notebook
</commit_message>
<xml_diff>
--- a/RequiredData.xlsx
+++ b/RequiredData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\RMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS\projects\k2s-hotel-reservation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40DBC16-095A-43AA-AD43-ADEE0B46C7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E6E8A4-11AC-4209-AAB4-1A8CB4228A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{5AF43ABF-52C1-4D51-A72D-F9A2FF35AFE0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5AF43ABF-52C1-4D51-A72D-F9A2FF35AFE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Reservation List" sheetId="1" r:id="rId1"/>
@@ -92,8 +92,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -130,22 +130,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -170,10 +170,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,20 +471,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C82A3B-34EA-4544-8416-E855CDB8C294}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" customWidth="1"/>
-    <col min="2" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" customWidth="1"/>
-    <col min="7" max="7" width="11.08984375" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="91.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
@@ -514,7 +510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -538,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -562,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -586,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -612,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -636,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -662,58 +658,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="E16" s="3"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
     </row>
   </sheetData>
@@ -730,13 +726,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -744,7 +740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>44927</v>
       </c>
@@ -752,7 +748,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -760,7 +756,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>45047</v>
       </c>
@@ -768,7 +764,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>45178</v>
       </c>
@@ -776,7 +772,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -784,7 +780,7 @@
         <v>40500</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -801,17 +797,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CD88A9-4437-42D6-AF41-5F206A2F8B48}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="117" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -819,7 +815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>45017</v>
       </c>
@@ -827,7 +823,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>45018</v>
       </c>
@@ -835,7 +831,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>45019</v>
       </c>
@@ -843,7 +839,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>45020</v>
       </c>
@@ -851,7 +847,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>45021</v>
       </c>
@@ -859,7 +855,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>45022</v>
       </c>
@@ -867,7 +863,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>45023</v>
       </c>
@@ -875,7 +871,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>45024</v>
       </c>
@@ -883,7 +879,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>45025</v>
       </c>
@@ -891,7 +887,7 @@
         <v>2825</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>45026</v>
       </c>
@@ -899,7 +895,7 @@
         <v>2825</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>45027</v>
       </c>
@@ -907,7 +903,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>45028</v>
       </c>
@@ -915,7 +911,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>45029</v>
       </c>

</xml_diff>

<commit_message>
made filtered df in util, and almost completed cash-flow
</commit_message>
<xml_diff>
--- a/RequiredData.xlsx
+++ b/RequiredData.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS\projects\k2s-hotel-reservation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C739A830-3F97-4DD5-A730-2AC007480ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Reservation List" sheetId="1" r:id="rId1"/>
-    <sheet name="Payment List" sheetId="2" r:id="rId2"/>
-    <sheet name="Total Avalibility" sheetId="3" r:id="rId3"/>
+    <sheet r:id="rId1" sheetId="1" name="Reservation List"/>
+    <sheet r:id="rId2" sheetId="2" name="Payment List"/>
+    <sheet r:id="rId3" sheetId="3" name="Total Avalibility"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -36,16 +30,10 @@
     <t>Payment Amount</t>
   </si>
   <si>
-    <t>14/1/2023</t>
-  </si>
-  <si>
-    <t>25/12/2023</t>
-  </si>
-  <si>
-    <t>15/3/2023</t>
-  </si>
-  <si>
     <t>Reservation ID</t>
+  </si>
+  <si>
+    <t>Reservation Creation Date (MM-DD-YYYY)</t>
   </si>
   <si>
     <t>Reservation Check-in Date</t>
@@ -65,22 +53,16 @@
   <si>
     <t>Type
 allotment (1),  sales allotment (2), direct hotel (3)or direct agent(4)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Reservation Creation Date (MM-DD-YYYY)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +73,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -122,68 +110,89 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+  <cellXfs count="25">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -194,10 +203,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -235,71 +244,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -327,7 +336,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -350,11 +359,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -363,13 +372,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -379,7 +388,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -388,7 +397,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -397,7 +406,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -405,10 +414,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -473,53 +482,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.44140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="21" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="22" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="23" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="23" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="24" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="21" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="23" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="21" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="88.5" customFormat="1" s="9">
+      <c r="A1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -532,10 +541,10 @@
       <c r="D2" s="3">
         <v>45058</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="7">
         <v>24000</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="13">
         <v>10</v>
       </c>
       <c r="G2" s="3"/>
@@ -543,7 +552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -556,10 +565,10 @@
       <c r="D3" s="3">
         <v>45055</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="7">
         <v>5000</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="13">
         <v>5</v>
       </c>
       <c r="G3" s="3"/>
@@ -567,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -580,10 +589,10 @@
       <c r="D4" s="3">
         <v>45148</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="7">
         <v>200</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="13">
         <v>5</v>
       </c>
       <c r="G4" s="3">
@@ -593,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -606,10 +615,10 @@
       <c r="D5" s="3">
         <v>45185</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="7">
         <v>7200</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="13">
         <v>4</v>
       </c>
       <c r="G5" s="3">
@@ -619,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -632,10 +641,10 @@
       <c r="D6" s="3">
         <v>44938</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="7">
         <v>81400</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="13">
         <v>20</v>
       </c>
       <c r="G6" s="3"/>
@@ -643,7 +652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -656,73 +665,126 @@
       <c r="D7" s="3">
         <v>45043</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="7">
         <v>74243</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="13">
         <v>55</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="16"/>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="14"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
-      <c r="C14" s="18"/>
-      <c r="E14" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
-      <c r="C15" s="18"/>
-      <c r="E15" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="E16" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="14"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -730,73 +792,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="15.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>44927</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="7">
         <v>12000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="3">
+        <v>44940</v>
+      </c>
+      <c r="B3" s="7">
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
-        <v>45047</v>
-      </c>
-      <c r="B4" s="5">
+        <v>44931</v>
+      </c>
+      <c r="B4" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>45178</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="7">
         <v>7200</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="3">
+        <v>45285</v>
+      </c>
+      <c r="B6" s="7">
         <v>40500</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="3">
+        <v>45000</v>
+      </c>
+      <c r="B7" s="7">
         <v>37225</v>
       </c>
     </row>
@@ -806,7 +868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -814,13 +876,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="16.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,7 +890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>45017</v>
       </c>
@@ -836,7 +898,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>45018</v>
       </c>
@@ -844,7 +906,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>45019</v>
       </c>
@@ -852,7 +914,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>45020</v>
       </c>
@@ -860,7 +922,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>45021</v>
       </c>
@@ -868,7 +930,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>45022</v>
       </c>
@@ -876,7 +938,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>45023</v>
       </c>
@@ -884,7 +946,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>45024</v>
       </c>
@@ -892,7 +954,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>45025</v>
       </c>
@@ -900,7 +962,7 @@
         <v>2825</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>45026</v>
       </c>
@@ -908,7 +970,7 @@
         <v>2825</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
         <v>45027</v>
       </c>
@@ -916,7 +978,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3">
         <v>45028</v>
       </c>
@@ -924,7 +986,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3">
         <v>45029</v>
       </c>

</xml_diff>

<commit_message>
finished data preparation (on DUMMY DATA) for cash-flow and util-res
</commit_message>
<xml_diff>
--- a/RequiredData.xlsx
+++ b/RequiredData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Reservation List"/>
@@ -62,19 +62,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -110,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -118,19 +112,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -139,50 +127,32 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,303 +458,303 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="21" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="22" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="23" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="23" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="24" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="21" width="7.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="23" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="21" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="15" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="15" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="88.5" customFormat="1" s="9">
-      <c r="A1" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="88.5" customFormat="1" s="7">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>44927</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>45047</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>45058</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <v>24000</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="11">
         <v>10</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4">
+      <c r="G2" s="1"/>
+      <c r="H2" s="2">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>44927</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>45050</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>45055</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>5000</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="11">
         <v>5</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4">
+      <c r="G3" s="1"/>
+      <c r="H3" s="2">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>44927</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>45147</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>45148</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>200</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="11">
         <v>5</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="1">
         <v>44929</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>44928</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>45176</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>45185</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>7200</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="11">
         <v>4</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="1">
         <v>44929</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="2">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>44928</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>44935</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>44938</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>81400</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="11">
         <v>20</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4">
+      <c r="G6" s="1"/>
+      <c r="H6" s="2">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>44929</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>45037</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>45043</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>74243</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="11">
         <v>55</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4">
+      <c r="G7" s="1"/>
+      <c r="H7" s="2">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="14"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="14"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="14"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="14"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="14"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="14"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="14"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="14"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="14"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="14"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="14"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="14"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -798,67 +768,67 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="15.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>44927</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>12000</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>44940</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>3000</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>44931</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>200</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>45178</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>7200</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>45285</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>40500</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>45000</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>37225</v>
       </c>
     </row>
@@ -878,8 +848,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="16.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -891,106 +861,106 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>45017</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>2700</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>45018</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>2700</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>45019</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>2700</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>45020</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>2700</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>45021</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="2">
         <v>2700</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>45022</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>2750</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <v>45023</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>2750</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="3">
+      <c r="A9" s="1">
         <v>45024</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="2">
         <v>2750</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <v>45025</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="2">
         <v>2825</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="3">
+      <c r="A11" s="1">
         <v>45026</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="2">
         <v>2825</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="3">
+      <c r="A12" s="1">
         <v>45027</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="2">
         <v>2900</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="3">
+      <c r="A13" s="1">
         <v>45028</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>2800</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="3">
+      <c r="A14" s="1">
         <v>45029</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="2">
         <v>2850</v>
       </c>
     </row>

</xml_diff>